<commit_message>
fixed dcf to work with Q data, messing with goal seek
</commit_message>
<xml_diff>
--- a/southwest.xlsx
+++ b/southwest.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="14560" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="14560" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="7" r:id="rId1"/>
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="517">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="517">
   <si>
     <t>Company Name</t>
   </si>
@@ -4098,19 +4098,19 @@
                 <c:formatCode>_-* #,##0_-;\(#,##0\)_-;_-* "-"_-;_-@_-</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>3521.6616273462</c:v>
+                  <c:v>3368.851756135782</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4236.446642509325</c:v>
+                  <c:v>4443.78950166004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4878.122362049653</c:v>
+                  <c:v>5690.12875952076</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5650.68169188151</c:v>
+                  <c:v>7003.03200877302</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5750.655654817943</c:v>
+                  <c:v>8430.156307418145</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6894,7 +6894,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="57" dropStyle="combo" dx="16" fmlaLink="$L$4" fmlaRange="$D$4:$D$6" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="56" dropStyle="combo" dx="16" fmlaLink="$L$4" fmlaRange="$D$4:$D$6" sel="2" val="0"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13006,18 +13006,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W252"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D135" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="3" ySplit="3" topLeftCell="F31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D122" sqref="D122"/>
+      <selection pane="bottomRight" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" outlineLevelRow="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.6640625" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="30.83203125" customWidth="1"/>
     <col min="4" max="18" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -13387,7 +13387,7 @@
       <c r="L9" s="280"/>
       <c r="M9" s="396">
         <f>Scenarios!I9</f>
-        <v>2.5000000000000001E-2</v>
+        <v>-2.2672178274219957E-2</v>
       </c>
       <c r="N9" s="396">
         <f>Scenarios!J9</f>
@@ -13435,23 +13435,23 @@
       <c r="L10" s="435"/>
       <c r="M10" s="394">
         <f>Scenarios!I10</f>
-        <v>163790031.82499999</v>
+        <v>156172248.80382773</v>
       </c>
       <c r="N10" s="394">
         <f>Scenarios!J10</f>
-        <v>167884782.62062496</v>
+        <v>160076555.02392343</v>
       </c>
       <c r="O10" s="394">
         <f>Scenarios!K10</f>
-        <v>172081902.18614057</v>
+        <v>164078468.8995215</v>
       </c>
       <c r="P10" s="394">
         <f>Scenarios!L10</f>
-        <v>176383949.74079406</v>
+        <v>168180430.62200952</v>
       </c>
       <c r="Q10" s="394">
         <f>Scenarios!M10</f>
-        <v>180793548.48431391</v>
+        <v>172384941.38755974</v>
       </c>
       <c r="R10" s="64"/>
       <c r="S10" s="64">
@@ -13529,23 +13529,23 @@
       <c r="L12" s="134"/>
       <c r="M12" s="392">
         <f>Scenarios!I12</f>
-        <v>13.375999999999999</v>
+        <v>12.750194552529186</v>
       </c>
       <c r="N12" s="392">
         <f>Scenarios!J12</f>
-        <v>13.977919999999999</v>
+        <v>12.700582900573821</v>
       </c>
       <c r="O12" s="392">
         <f>Scenarios!K12</f>
-        <v>14.606926399999999</v>
+        <v>12.651164290065752</v>
       </c>
       <c r="P12" s="392">
         <f>Scenarios!L12</f>
-        <v>15.264238087999997</v>
+        <v>12.601937969870946</v>
       </c>
       <c r="Q12" s="392">
         <f>Scenarios!M12</f>
-        <v>15.951128801959996</v>
+        <v>12.552903191778064</v>
       </c>
       <c r="R12" s="64"/>
       <c r="S12" s="64">
@@ -13579,19 +13579,19 @@
       </c>
       <c r="N13" s="392">
         <f>Scenarios!J13</f>
-        <v>11.7</v>
+        <v>11.394131071458736</v>
       </c>
       <c r="O13" s="392">
         <f>Scenarios!K13</f>
-        <v>12</v>
+        <v>11.225036660753679</v>
       </c>
       <c r="P13" s="392">
         <f>Scenarios!L13</f>
-        <v>12.25</v>
+        <v>11.058451692809319</v>
       </c>
       <c r="Q13" s="392">
         <f>Scenarios!M13</f>
-        <v>13</v>
+        <v>10.894338926282531</v>
       </c>
       <c r="R13" s="64"/>
       <c r="S13" s="64">
@@ -13671,19 +13671,19 @@
       </c>
       <c r="N15" s="392">
         <f>Scenarios!J15</f>
-        <v>2.2000000000000002</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="O15" s="392">
         <f>Scenarios!K15</f>
-        <v>2.2999999999999998</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="P15" s="392">
         <f>Scenarios!L15</f>
-        <v>2.15</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="Q15" s="392">
         <f>Scenarios!M15</f>
-        <v>2.2999999999999998</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="R15" s="64"/>
       <c r="S15" s="64">
@@ -13957,7 +13957,7 @@
       </c>
       <c r="L20" s="425">
         <f t="shared" si="6"/>
-        <v>0.19998710601299002</v>
+        <v>0.19895551520995619</v>
       </c>
       <c r="M20" s="389">
         <f>Scenarios!I20</f>
@@ -14024,7 +14024,7 @@
       </c>
       <c r="L21" s="70">
         <f t="shared" si="7"/>
-        <v>40.350590853155651</v>
+        <v>47.088194323524313</v>
       </c>
       <c r="M21" s="394">
         <f>Scenarios!I21</f>
@@ -14091,7 +14091,7 @@
       </c>
       <c r="L22" s="429">
         <f t="shared" si="8"/>
-        <v>10.085679970374928</v>
+        <v>12.241975355504058</v>
       </c>
       <c r="M22" s="393">
         <f>Scenarios!I22</f>
@@ -14154,7 +14154,7 @@
       </c>
       <c r="L23" s="70">
         <f t="shared" si="9"/>
-        <v>118.10413528423967</v>
+        <v>115.17718380303651</v>
       </c>
       <c r="M23" s="394">
         <f>Scenarios!I23</f>
@@ -14217,7 +14217,7 @@
       </c>
       <c r="L24" s="70">
         <f t="shared" si="10"/>
-        <v>27.641115512772998</v>
+        <v>33.44949761900935</v>
       </c>
       <c r="M24" s="394">
         <f>Scenarios!I24</f>
@@ -14653,7 +14653,7 @@
       <c r="L31" s="280"/>
       <c r="M31" s="280">
         <f>M43/H43-1</f>
-        <v>7.1458238008408115E-2</v>
+        <v>2.1625312997951118E-2</v>
       </c>
       <c r="N31" s="280">
         <f>N43/M43-1</f>
@@ -14701,23 +14701,23 @@
       <c r="L32" s="78"/>
       <c r="M32" s="78">
         <f>M40/H40-1</f>
-        <v>7.1061092980298168E-2</v>
+        <v>-2.6533094131118595E-2</v>
       </c>
       <c r="N32" s="78">
         <f>N40/M40-1</f>
-        <v>7.1124999999999883E-2</v>
+        <v>2.101167315175112E-2</v>
       </c>
       <c r="O32" s="78">
         <f>O40/N40-1</f>
-        <v>7.1124999999999883E-2</v>
+        <v>2.101167315175112E-2</v>
       </c>
       <c r="P32" s="78">
         <f>P40/O40-1</f>
-        <v>7.1124999999999661E-2</v>
+        <v>2.1011673151750898E-2</v>
       </c>
       <c r="Q32" s="78">
         <f>Q40/P40-1</f>
-        <v>7.1124999999999883E-2</v>
+        <v>2.101167315175112E-2</v>
       </c>
     </row>
     <row r="33" spans="1:17" ht="16" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -14749,23 +14749,23 @@
       <c r="L33" s="78"/>
       <c r="M33" s="78">
         <f>M53/H53-1</f>
-        <v>9.8396945896457311E-3</v>
+        <v>-3.7127386336072599E-2</v>
       </c>
       <c r="N33" s="78">
         <f>N53/M53-1</f>
-        <v>3.6895699300836693E-2</v>
+        <v>9.7885047235555245E-3</v>
       </c>
       <c r="O33" s="78">
         <f>O53/N53-1</f>
-        <v>5.1282051282051322E-2</v>
+        <v>9.7885047235553024E-3</v>
       </c>
       <c r="P33" s="78">
         <f>P53/O53-1</f>
-        <v>4.6354166666666474E-2</v>
+        <v>9.7885047235555245E-3</v>
       </c>
       <c r="Q33" s="78">
         <f>Q53/P53-1</f>
-        <v>8.7755102040816269E-2</v>
+        <v>9.7885047235555245E-3</v>
       </c>
     </row>
     <row r="34" spans="1:17" ht="17" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -14976,27 +14976,27 @@
       </c>
       <c r="L40" s="282">
         <f>M40-SUM(I40:K40)</f>
-        <v>6446.5546569119979</v>
+        <v>4450.26555954797</v>
       </c>
       <c r="M40" s="109">
         <f>M12*M10/100000</f>
-        <v>21908.554656911998</v>
+        <v>19912.26555954797</v>
       </c>
       <c r="N40" s="109">
         <f>N12*N10/100000</f>
-        <v>23466.800606884863</v>
+        <v>20330.655575196062</v>
       </c>
       <c r="O40" s="109">
         <f>O12*O10/100000</f>
-        <v>25135.876800049544</v>
+        <v>20757.836665102906</v>
       </c>
       <c r="P40" s="109">
         <f>P12*P10/100000</f>
-        <v>26923.666037453058</v>
+        <v>21193.99354444748</v>
       </c>
       <c r="Q40" s="109">
         <f>Q12*Q10/100000</f>
-        <v>28838.611784366902</v>
+        <v>21639.314809583731</v>
       </c>
     </row>
     <row r="41" spans="1:17" ht="16" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -15081,27 +15081,27 @@
       </c>
       <c r="L42" s="285">
         <f t="shared" si="21"/>
-        <v>344.02554094268635</v>
+        <v>1245.7344404520263</v>
       </c>
       <c r="M42" s="95">
         <f>M43-M39-M40</f>
-        <v>1451.0255409426863</v>
+        <v>2352.7344404520263</v>
       </c>
       <c r="N42" s="95">
         <f t="shared" ref="N42:Q42" si="22">N43-N39-N40</f>
-        <v>1566.6766075422311</v>
+        <v>3530.3894248039323</v>
       </c>
       <c r="O42" s="95">
         <f t="shared" si="22"/>
-        <v>1690.553356253673</v>
+        <v>4812.7720355220845</v>
       </c>
       <c r="P42" s="95">
         <f t="shared" si="22"/>
-        <v>1823.2408387172145</v>
+        <v>6207.771575009454</v>
       </c>
       <c r="Q42" s="95">
         <f t="shared" si="22"/>
-        <v>1965.3657183709765</v>
+        <v>7723.8477289945731</v>
       </c>
     </row>
     <row r="43" spans="1:17" ht="16" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -15144,27 +15144,27 @@
       </c>
       <c r="L43" s="283">
         <f>SUM(L39:L42)</f>
-        <v>6837.5801978546842</v>
+        <v>5742.9999999999964</v>
       </c>
       <c r="M43" s="86">
         <f>M10*M11/100000</f>
-        <v>23534.580197854684</v>
+        <v>22439.999999999996</v>
       </c>
       <c r="N43" s="86">
         <f>N10*N11/100000</f>
-        <v>25208.477214427094</v>
+        <v>24036.044999999995</v>
       </c>
       <c r="O43" s="86">
         <f>O10*O11/100000</f>
-        <v>27001.430156303217</v>
+        <v>25745.608700624991</v>
       </c>
       <c r="P43" s="86">
         <f>P10*P11/100000</f>
-        <v>28921.906876170273</v>
+        <v>27576.765119456933</v>
       </c>
       <c r="Q43" s="86">
         <f>Q10*Q11/100000</f>
-        <v>30978.977502737878</v>
+        <v>29538.162538578305</v>
       </c>
     </row>
     <row r="44" spans="1:17" ht="16" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -15560,27 +15560,27 @@
       </c>
       <c r="L53" s="297">
         <f t="shared" si="21"/>
-        <v>4538.582830807165</v>
+        <v>3657.5273597216146</v>
       </c>
       <c r="M53" s="321">
         <f>M10*M13/100000</f>
-        <v>18943.582830807165</v>
+        <v>18062.527359721615</v>
       </c>
       <c r="N53" s="321">
         <f>N10*N13/100000</f>
-        <v>19642.519566613119</v>
+        <v>18239.3324941016</v>
       </c>
       <c r="O53" s="321">
         <f>O10*O13/100000</f>
-        <v>20649.828262336869</v>
+        <v>18417.868286374611</v>
       </c>
       <c r="P53" s="321">
         <f>P10*P13/100000</f>
-        <v>21607.033843247271</v>
+        <v>18598.151677093614</v>
       </c>
       <c r="Q53" s="321">
         <f>Q10*Q13/100000</f>
-        <v>23503.161302960805</v>
+        <v>18780.199772634245</v>
       </c>
     </row>
     <row r="54" spans="1:17" ht="16" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -15888,27 +15888,27 @@
       </c>
       <c r="L59" s="86">
         <f>SUM(L53:L58)</f>
-        <v>4551.5278308071647</v>
+        <v>3670.4723597216148</v>
       </c>
       <c r="M59" s="86">
         <f t="shared" si="32"/>
-        <v>18957.527830807165</v>
+        <v>18076.472359721614</v>
       </c>
       <c r="N59" s="86">
         <f t="shared" si="32"/>
-        <v>19693.547899946454</v>
+        <v>18290.360827434935</v>
       </c>
       <c r="O59" s="86">
         <f t="shared" si="32"/>
-        <v>20669.189929003533</v>
+        <v>18437.229953041275</v>
       </c>
       <c r="P59" s="86">
         <f t="shared" si="32"/>
-        <v>21629.103843247271</v>
+        <v>18620.221677093614</v>
       </c>
       <c r="Q59" s="86">
         <f t="shared" si="32"/>
-        <v>23510.752136294141</v>
+        <v>18787.790605967581</v>
       </c>
     </row>
     <row r="60" spans="1:17" ht="16" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -15951,27 +15951,27 @@
       </c>
       <c r="L60" s="89">
         <f>L43-L59</f>
-        <v>2286.0523670475195</v>
+        <v>2072.5276402783816</v>
       </c>
       <c r="M60" s="89">
         <f>M43-M59</f>
-        <v>4577.0523670475195</v>
+        <v>4363.527640278382</v>
       </c>
       <c r="N60" s="89">
         <f t="shared" ref="N60:Q60" si="40">N43-N59</f>
-        <v>5514.9293144806397</v>
+        <v>5745.6841725650593</v>
       </c>
       <c r="O60" s="89">
         <f t="shared" si="40"/>
-        <v>6332.2402272996842</v>
+        <v>7308.3787475837162</v>
       </c>
       <c r="P60" s="89">
         <f t="shared" si="40"/>
-        <v>7292.8030329230023</v>
+        <v>8956.5434423633196</v>
       </c>
       <c r="Q60" s="89">
         <f t="shared" si="40"/>
-        <v>7468.2253664437376</v>
+        <v>10750.371932610724</v>
       </c>
     </row>
     <row r="61" spans="1:17" ht="16" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
@@ -16006,27 +16006,27 @@
       </c>
       <c r="L61" s="88">
         <f t="shared" si="21"/>
-        <v>457.18099707997908</v>
+        <v>412.34080445846018</v>
       </c>
       <c r="M61" s="96">
         <f>M60*M20</f>
-        <v>961.18099707997908</v>
+        <v>916.34080445846018</v>
       </c>
       <c r="N61" s="96">
         <f>N60*N20</f>
-        <v>1158.1351560409344</v>
+        <v>1206.5936762386625</v>
       </c>
       <c r="O61" s="96">
         <f>O60*O20</f>
-        <v>1329.7704477329337</v>
+        <v>1534.7595369925803</v>
       </c>
       <c r="P61" s="96">
         <f>P60*P20</f>
-        <v>1531.4886369138305</v>
+        <v>1880.874122896297</v>
       </c>
       <c r="Q61" s="96">
         <f>Q60*Q20</f>
-        <v>1568.3273269531849</v>
+        <v>2257.5781058482521</v>
       </c>
     </row>
     <row r="62" spans="1:17" ht="17" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -16069,27 +16069,27 @@
       </c>
       <c r="L62" s="99">
         <f>L60-L61</f>
-        <v>1828.8713699675404</v>
+        <v>1660.1868358199213</v>
       </c>
       <c r="M62" s="99">
         <f>M60-M61</f>
-        <v>3615.8713699675404</v>
+        <v>3447.1868358199217</v>
       </c>
       <c r="N62" s="99">
         <f>N60-N61</f>
-        <v>4356.7941584397049</v>
+        <v>4539.0904963263965</v>
       </c>
       <c r="O62" s="99">
         <f>O60-O61</f>
-        <v>5002.4697795667507</v>
+        <v>5773.6192105911359</v>
       </c>
       <c r="P62" s="99">
         <f>P60-P61</f>
-        <v>5761.314396009172</v>
+        <v>7075.6693194670224</v>
       </c>
       <c r="Q62" s="99">
         <f>Q60-Q61</f>
-        <v>5899.8980394905529</v>
+        <v>8492.7938267624722</v>
       </c>
     </row>
     <row r="63" spans="1:17" ht="17" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.2">
@@ -16308,27 +16308,27 @@
       </c>
       <c r="L73" s="64">
         <f>M73</f>
-        <v>4670.242662588882</v>
+        <v>4485.6834655040602</v>
       </c>
       <c r="M73" s="64">
         <f>M162</f>
-        <v>4670.242662588882</v>
+        <v>4485.6834655040602</v>
       </c>
       <c r="N73" s="64">
         <f t="shared" ref="N73:Q73" si="41">N162</f>
-        <v>8010.7036647367458</v>
+        <v>7983.3942842745901</v>
       </c>
       <c r="O73" s="64">
         <f t="shared" si="41"/>
-        <v>12122.449727407013</v>
+        <v>12825.432811522522</v>
       </c>
       <c r="P73" s="64">
         <f t="shared" si="41"/>
-        <v>17108.754062396809</v>
+        <v>19088.096676536516</v>
       </c>
       <c r="Q73" s="64">
         <f t="shared" si="41"/>
-        <v>22375.199975255106</v>
+        <v>26860.833511338453</v>
       </c>
     </row>
     <row r="74" spans="1:20" ht="16" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -16419,27 +16419,27 @@
       </c>
       <c r="L75" s="64">
         <f t="shared" si="42"/>
-        <v>644.78301911930646</v>
+        <v>614.79452054794513</v>
       </c>
       <c r="M75" s="64">
         <f>M43/365*M21</f>
-        <v>644.78301911930646</v>
+        <v>614.79452054794513</v>
       </c>
       <c r="N75" s="64">
         <f>N43/365*N21</f>
-        <v>690.64321135416685</v>
+        <v>658.52178082191767</v>
       </c>
       <c r="O75" s="64">
         <f>O43/365*O21</f>
-        <v>739.76520976173197</v>
+        <v>705.35914248287645</v>
       </c>
       <c r="P75" s="64">
         <f>P43/365*P21</f>
-        <v>792.38101030603491</v>
+        <v>755.52781149197074</v>
       </c>
       <c r="Q75" s="64">
         <f>Q43/365*Q21</f>
-        <v>848.73910966405151</v>
+        <v>809.2647270843371</v>
       </c>
       <c r="R75" s="323"/>
     </row>
@@ -16475,27 +16475,27 @@
       </c>
       <c r="L76" s="64">
         <f t="shared" si="42"/>
-        <v>467.10204240346434</v>
+        <v>445.37738695203984</v>
       </c>
       <c r="M76" s="64">
         <f>M53/365*M22</f>
-        <v>467.10204240346434</v>
+        <v>445.37738695203984</v>
       </c>
       <c r="N76" s="64">
         <f>N53/365*N22</f>
-        <v>484.33609890278922</v>
+        <v>449.73696560798464</v>
       </c>
       <c r="O76" s="64">
         <f>O53/365*O22</f>
-        <v>509.17384756447075</v>
+        <v>454.13921802019593</v>
       </c>
       <c r="P76" s="64">
         <f>P53/365*P22</f>
-        <v>532.77617695678202</v>
+        <v>458.58456190093841</v>
       </c>
       <c r="Q76" s="64">
         <f>Q53/365*Q22</f>
-        <v>579.53000473054044</v>
+        <v>463.07341905125531</v>
       </c>
       <c r="R76" s="323"/>
     </row>
@@ -16595,27 +16595,27 @@
       </c>
       <c r="L78" s="104">
         <f t="shared" si="42"/>
-        <v>7927.1277241116522</v>
+        <v>7690.8553730040458</v>
       </c>
       <c r="M78" s="104">
         <f>SUM(M73:M77)</f>
-        <v>7927.1277241116522</v>
+        <v>7690.8553730040458</v>
       </c>
       <c r="N78" s="104">
         <f t="shared" si="45"/>
-        <v>11330.682974993702</v>
+        <v>11236.65303070449</v>
       </c>
       <c r="O78" s="104">
         <f t="shared" si="45"/>
-        <v>15516.388784733215</v>
+        <v>16129.931172025596</v>
       </c>
       <c r="P78" s="104">
         <f t="shared" si="45"/>
-        <v>20578.911249659624</v>
+        <v>22447.209049929425</v>
       </c>
       <c r="Q78" s="104">
         <f t="shared" si="45"/>
-        <v>25948.469089649698</v>
+        <v>30278.171657474046</v>
       </c>
       <c r="R78" s="323"/>
     </row>
@@ -17155,27 +17155,27 @@
       </c>
       <c r="L90" s="99">
         <f t="shared" si="42"/>
-        <v>29368.47772411165</v>
+        <v>29132.205373004042</v>
       </c>
       <c r="M90" s="99">
         <f>SUM(M84:M88)+M78</f>
-        <v>29368.47772411165</v>
+        <v>29132.205373004042</v>
       </c>
       <c r="N90" s="99">
         <f t="shared" ref="N90" si="56">SUM(N84:N88)+N78</f>
-        <v>32981.4067249937</v>
+        <v>32887.376780704486</v>
       </c>
       <c r="O90" s="99">
         <f t="shared" ref="O90" si="57">SUM(O84:O88)+O78</f>
-        <v>37360.783253483212</v>
+        <v>37974.325640775591</v>
       </c>
       <c r="P90" s="99">
         <f t="shared" ref="P90" si="58">SUM(P84:P88)+P78</f>
-        <v>42602.451133253373</v>
+        <v>44470.748933523173</v>
       </c>
       <c r="Q90" s="99">
         <f t="shared" ref="Q90" si="59">SUM(Q84:Q88)+Q78</f>
-        <v>48137.71848197392</v>
+        <v>52467.421049798264</v>
       </c>
       <c r="R90" s="323"/>
     </row>
@@ -17259,27 +17259,27 @@
       </c>
       <c r="L93" s="76">
         <f t="shared" si="42"/>
-        <v>1453.2063541441112</v>
+        <v>1385.6185371841239</v>
       </c>
       <c r="M93" s="76">
         <f>M53/365*M24</f>
-        <v>1453.2063541441112</v>
+        <v>1385.6185371841239</v>
       </c>
       <c r="N93" s="76">
         <f>N53/365*N24</f>
-        <v>1506.8234188086776</v>
+        <v>1399.1816707803969</v>
       </c>
       <c r="O93" s="76">
         <f>O53/365*O24</f>
-        <v>1584.0964146450201</v>
+        <v>1412.8775671739427</v>
       </c>
       <c r="P93" s="76">
         <f>P53/365*P24</f>
-        <v>1657.5258838655441</v>
+        <v>1426.7075259140306</v>
       </c>
       <c r="Q93" s="76">
         <f>Q53/365*Q24</f>
-        <v>1802.982236939459</v>
+        <v>1440.6728592705722</v>
       </c>
       <c r="R93" s="323"/>
     </row>
@@ -17522,27 +17522,27 @@
       </c>
       <c r="L98" s="104">
         <f t="shared" si="42"/>
-        <v>8544.0063541441123</v>
+        <v>8476.4185371841249</v>
       </c>
       <c r="M98" s="104">
         <f t="shared" si="61"/>
-        <v>8544.0063541441123</v>
+        <v>8476.4185371841249</v>
       </c>
       <c r="N98" s="104">
         <f t="shared" si="61"/>
-        <v>8860.1411965864572</v>
+        <v>8752.4994485581756</v>
       </c>
       <c r="O98" s="104">
         <f t="shared" si="61"/>
-        <v>9297.0479455092191</v>
+        <v>9125.8290980381425</v>
       </c>
       <c r="P98" s="104">
         <f t="shared" si="61"/>
-        <v>9837.4014292702104</v>
+        <v>9606.583071318697</v>
       </c>
       <c r="Q98" s="104">
         <f t="shared" si="61"/>
-        <v>10532.7707385002</v>
+        <v>10170.461360831314</v>
       </c>
       <c r="R98" s="323"/>
     </row>
@@ -17925,27 +17925,27 @@
       </c>
       <c r="L106" s="104">
         <f t="shared" si="42"/>
-        <v>16759.606354144111</v>
+        <v>16692.018537184125</v>
       </c>
       <c r="M106" s="104">
         <f>SUM(M100:M104)+M98</f>
-        <v>16759.606354144111</v>
+        <v>16692.018537184125</v>
       </c>
       <c r="N106" s="104">
         <f>SUM(N100:N104)+N98</f>
-        <v>16875.741196586459</v>
+        <v>16768.099448558176</v>
       </c>
       <c r="O106" s="104">
         <f>SUM(O100:O104)+O98</f>
-        <v>17112.647945509219</v>
+        <v>16941.429098038141</v>
       </c>
       <c r="P106" s="104">
         <f>SUM(P100:P104)+P98</f>
-        <v>17453.001429270211</v>
+        <v>17222.183071318697</v>
       </c>
       <c r="Q106" s="104">
         <f>SUM(Q100:Q104)+Q98</f>
-        <v>17948.370738500198</v>
+        <v>17586.061360831314</v>
       </c>
       <c r="R106" s="323"/>
     </row>
@@ -18174,27 +18174,27 @@
       </c>
       <c r="L111" s="92">
         <f t="shared" si="42"/>
-        <v>19222.871369967539</v>
+        <v>19054.186835819921</v>
       </c>
       <c r="M111" s="92">
         <f>H111+M62-(-M153)</f>
-        <v>19222.871369967539</v>
+        <v>19054.186835819921</v>
       </c>
       <c r="N111" s="92">
         <f>M111+N62-(-N153)</f>
-        <v>23219.665528407244</v>
+        <v>23233.277332146317</v>
       </c>
       <c r="O111" s="92">
         <f>N111+O62-(-O153)</f>
-        <v>27862.135307973993</v>
+        <v>28646.896542737453</v>
       </c>
       <c r="P111" s="92">
         <f>O111+P62-(-P153)</f>
-        <v>33263.449703983162</v>
+        <v>35362.565862204472</v>
       </c>
       <c r="Q111" s="92">
         <f>P111+Q62-(-Q153)</f>
-        <v>38803.347743473714</v>
+        <v>43495.359688966942</v>
       </c>
       <c r="R111" s="323"/>
     </row>
@@ -18294,27 +18294,27 @@
       </c>
       <c r="L113" s="104">
         <f t="shared" si="42"/>
-        <v>12608.871369967539</v>
+        <v>12440.186835819921</v>
       </c>
       <c r="M113" s="104">
         <f>SUM(M108:M112)</f>
-        <v>12608.871369967539</v>
+        <v>12440.186835819921</v>
       </c>
       <c r="N113" s="104">
         <f t="shared" si="68"/>
-        <v>16105.665528407244</v>
+        <v>16119.277332146317</v>
       </c>
       <c r="O113" s="104">
         <f t="shared" si="68"/>
-        <v>20248.135307973993</v>
+        <v>21032.896542737453</v>
       </c>
       <c r="P113" s="104">
         <f t="shared" si="68"/>
-        <v>25149.449703983162</v>
+        <v>27248.565862204472</v>
       </c>
       <c r="Q113" s="104">
         <f t="shared" si="68"/>
-        <v>30189.347743473714</v>
+        <v>34881.359688966942</v>
       </c>
       <c r="R113" s="323"/>
     </row>
@@ -18358,27 +18358,27 @@
       </c>
       <c r="L114" s="99">
         <f t="shared" si="42"/>
-        <v>29368.47772411165</v>
+        <v>29132.205373004046</v>
       </c>
       <c r="M114" s="99">
         <f>M106+M113</f>
-        <v>29368.47772411165</v>
+        <v>29132.205373004046</v>
       </c>
       <c r="N114" s="99">
         <f t="shared" si="70"/>
-        <v>32981.406724993707</v>
+        <v>32887.376780704493</v>
       </c>
       <c r="O114" s="99">
         <f t="shared" si="70"/>
-        <v>37360.783253483212</v>
+        <v>37974.325640775598</v>
       </c>
       <c r="P114" s="99">
         <f t="shared" si="70"/>
-        <v>42602.451133253373</v>
+        <v>44470.748933523166</v>
       </c>
       <c r="Q114" s="99">
         <f t="shared" si="70"/>
-        <v>48137.718481973912</v>
+        <v>52467.421049798257</v>
       </c>
       <c r="R114" s="323"/>
     </row>
@@ -18604,27 +18604,27 @@
       </c>
       <c r="L122" s="281">
         <f>M122-SUM(I122:K122)</f>
-        <v>1828.8713699675404</v>
+        <v>1660.1868358199217</v>
       </c>
       <c r="M122" s="286">
         <f>M62</f>
-        <v>3615.8713699675404</v>
+        <v>3447.1868358199217</v>
       </c>
       <c r="N122" s="286">
         <f>N62</f>
-        <v>4356.7941584397049</v>
+        <v>4539.0904963263965</v>
       </c>
       <c r="O122" s="286">
         <f>O62</f>
-        <v>5002.4697795667507</v>
+        <v>5773.6192105911359</v>
       </c>
       <c r="P122" s="286">
         <f>P62</f>
-        <v>5761.314396009172</v>
+        <v>7075.6693194670224</v>
       </c>
       <c r="Q122" s="286">
         <f>Q62</f>
-        <v>5899.8980394905529</v>
+        <v>8492.7938267624722</v>
       </c>
     </row>
     <row r="123" spans="1:18" ht="16" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -19151,27 +19151,27 @@
       <c r="K136" s="281"/>
       <c r="L136" s="281">
         <f t="shared" si="74"/>
-        <v>-45.67870737865951</v>
+        <v>-61.55337031586123</v>
       </c>
       <c r="M136" s="286">
         <f>M175</f>
-        <v>-45.67870737865951</v>
+        <v>-61.55337031586123</v>
       </c>
       <c r="N136" s="286">
         <f t="shared" ref="N136:Q136" si="78">N175</f>
-        <v>-9.4771840696189429</v>
+        <v>-34.523705333644102</v>
       </c>
       <c r="O136" s="286">
         <f t="shared" si="78"/>
-        <v>3.3132487670959563</v>
+        <v>-37.543717679624478</v>
       </c>
       <c r="P136" s="286">
         <f t="shared" si="78"/>
-        <v>-2.7886607160903623</v>
+        <v>-40.784054149748727</v>
       </c>
       <c r="Q136" s="286">
         <f t="shared" si="78"/>
-        <v>42.344425942139878</v>
+        <v>-44.260439386141798</v>
       </c>
     </row>
     <row r="137" spans="1:17" ht="16" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -19214,27 +19214,27 @@
       </c>
       <c r="L137" s="287">
         <f t="shared" si="79"/>
-        <v>2263.2426625888816</v>
+        <v>2078.6834655040607</v>
       </c>
       <c r="M137" s="287">
         <f>SUM(M122:M136)</f>
-        <v>5426.242662588882</v>
+        <v>5241.6834655040602</v>
       </c>
       <c r="N137" s="287">
         <f t="shared" ref="N137:Q137" si="80">SUM(N122:N136)</f>
-        <v>5950.4610021478638</v>
+        <v>6107.7108187705298</v>
       </c>
       <c r="O137" s="287">
         <f t="shared" si="80"/>
-        <v>6721.7460626702668</v>
+        <v>7452.0385272479307</v>
       </c>
       <c r="P137" s="287">
         <f t="shared" si="80"/>
-        <v>7596.304334989798</v>
+        <v>8872.6638650139921</v>
       </c>
       <c r="Q137" s="287">
         <f t="shared" si="80"/>
-        <v>7876.4459128582985</v>
+        <v>10382.736834801935</v>
       </c>
     </row>
     <row r="138" spans="1:17" ht="16" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -19948,8 +19948,13 @@
       </c>
       <c r="I155" s="282"/>
       <c r="J155" s="282"/>
-      <c r="K155" s="282"/>
-      <c r="L155" s="281"/>
+      <c r="K155" s="282">
+        <v>0</v>
+      </c>
+      <c r="L155" s="281">
+        <f t="shared" si="85"/>
+        <v>0</v>
+      </c>
       <c r="M155" s="289"/>
       <c r="N155" s="289"/>
       <c r="O155" s="289"/>
@@ -19977,10 +19982,19 @@
       <c r="H156" s="282">
         <v>-30</v>
       </c>
-      <c r="I156" s="282"/>
-      <c r="J156" s="282"/>
-      <c r="K156" s="282"/>
-      <c r="L156" s="281"/>
+      <c r="I156" s="282">
+        <v>0</v>
+      </c>
+      <c r="J156" s="282">
+        <v>0</v>
+      </c>
+      <c r="K156" s="282">
+        <v>0</v>
+      </c>
+      <c r="L156" s="281">
+        <f t="shared" si="85"/>
+        <v>0</v>
+      </c>
       <c r="M156" s="289"/>
       <c r="N156" s="289"/>
       <c r="O156" s="289"/>
@@ -20008,10 +20022,19 @@
       <c r="H157" s="282">
         <v>170</v>
       </c>
-      <c r="I157" s="282"/>
-      <c r="J157" s="282"/>
-      <c r="K157" s="282"/>
-      <c r="L157" s="281"/>
+      <c r="I157" s="282" t="s">
+        <v>193</v>
+      </c>
+      <c r="J157" s="282">
+        <v>0</v>
+      </c>
+      <c r="K157" s="282">
+        <v>0</v>
+      </c>
+      <c r="L157" s="281">
+        <f t="shared" si="85"/>
+        <v>0</v>
+      </c>
       <c r="M157" s="289"/>
       <c r="N157" s="289"/>
       <c r="O157" s="289"/>
@@ -20140,27 +20163,27 @@
       </c>
       <c r="L160" s="296">
         <f t="shared" ref="L160" si="90">SUM(L158,L145,L137)</f>
-        <v>2182.2426625888816</v>
+        <v>1997.6834655040607</v>
       </c>
       <c r="M160" s="296">
         <f>SUM(M158,M145,M137)</f>
-        <v>2816.242662588882</v>
+        <v>2631.6834655040602</v>
       </c>
       <c r="N160" s="296">
         <f t="shared" si="88"/>
-        <v>3340.4610021478638</v>
+        <v>3497.7108187705298</v>
       </c>
       <c r="O160" s="296">
         <f t="shared" si="88"/>
-        <v>4111.7460626702668</v>
+        <v>4842.0385272479307</v>
       </c>
       <c r="P160" s="296">
         <f t="shared" si="88"/>
-        <v>4986.304334989798</v>
+        <v>6262.6638650139921</v>
       </c>
       <c r="Q160" s="296">
         <f t="shared" si="88"/>
-        <v>5266.4459128582985</v>
+        <v>7772.7368348019354</v>
       </c>
     </row>
     <row r="161" spans="1:17" ht="16" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -20210,19 +20233,19 @@
       </c>
       <c r="N161" s="297">
         <f t="shared" si="91"/>
-        <v>4670.242662588882</v>
+        <v>4485.6834655040602</v>
       </c>
       <c r="O161" s="297">
         <f t="shared" si="91"/>
-        <v>8010.7036647367458</v>
+        <v>7983.3942842745901</v>
       </c>
       <c r="P161" s="297">
         <f t="shared" si="91"/>
-        <v>12122.449727407013</v>
+        <v>12825.432811522522</v>
       </c>
       <c r="Q161" s="297">
         <f t="shared" si="91"/>
-        <v>17108.754062396809</v>
+        <v>19088.096676536516</v>
       </c>
     </row>
     <row r="162" spans="1:17" ht="16" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -20264,27 +20287,27 @@
       </c>
       <c r="L162" s="291">
         <f t="shared" ref="L162" si="93">SUM(L160:L161)</f>
-        <v>4670.242662588882</v>
+        <v>4485.6834655040602</v>
       </c>
       <c r="M162" s="291">
         <f>SUM(M160:M161)</f>
-        <v>4670.242662588882</v>
+        <v>4485.6834655040602</v>
       </c>
       <c r="N162" s="291">
         <f t="shared" si="92"/>
-        <v>8010.7036647367458</v>
+        <v>7983.3942842745901</v>
       </c>
       <c r="O162" s="291">
         <f t="shared" si="92"/>
-        <v>12122.449727407013</v>
+        <v>12825.432811522522</v>
       </c>
       <c r="P162" s="291">
         <f t="shared" si="92"/>
-        <v>17108.754062396809</v>
+        <v>19088.096676536516</v>
       </c>
       <c r="Q162" s="291">
         <f t="shared" si="92"/>
-        <v>22375.199975255106</v>
+        <v>26860.833511338453</v>
       </c>
     </row>
     <row r="163" spans="1:17" ht="16" x14ac:dyDescent="0.2">
@@ -20437,23 +20460,23 @@
       <c r="L169" s="91"/>
       <c r="M169" s="110">
         <f>M75</f>
-        <v>644.78301911930646</v>
+        <v>614.79452054794513</v>
       </c>
       <c r="N169" s="110">
         <f t="shared" ref="N169:Q169" si="94">N75</f>
-        <v>690.64321135416685</v>
+        <v>658.52178082191767</v>
       </c>
       <c r="O169" s="110">
         <f t="shared" si="94"/>
-        <v>739.76520976173197</v>
+        <v>705.35914248287645</v>
       </c>
       <c r="P169" s="110">
         <f t="shared" si="94"/>
-        <v>792.38101030603491</v>
+        <v>755.52781149197074</v>
       </c>
       <c r="Q169" s="110">
         <f t="shared" si="94"/>
-        <v>848.73910966405151</v>
+        <v>809.2647270843371</v>
       </c>
     </row>
     <row r="170" spans="1:17" ht="16" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -20488,23 +20511,23 @@
       <c r="L170" s="91"/>
       <c r="M170" s="110">
         <f>M76</f>
-        <v>467.10204240346434</v>
+        <v>445.37738695203984</v>
       </c>
       <c r="N170" s="110">
         <f t="shared" ref="N170:Q170" si="95">N76</f>
-        <v>484.33609890278922</v>
+        <v>449.73696560798464</v>
       </c>
       <c r="O170" s="110">
         <f t="shared" si="95"/>
-        <v>509.17384756447075</v>
+        <v>454.13921802019593</v>
       </c>
       <c r="P170" s="110">
         <f t="shared" si="95"/>
-        <v>532.77617695678202</v>
+        <v>458.58456190093841</v>
       </c>
       <c r="Q170" s="110">
         <f t="shared" si="95"/>
-        <v>579.53000473054044</v>
+        <v>463.07341905125531</v>
       </c>
     </row>
     <row r="171" spans="1:17" ht="16" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -20591,23 +20614,23 @@
       <c r="L172" s="91"/>
       <c r="M172" s="110">
         <f>M93</f>
-        <v>1453.2063541441112</v>
+        <v>1385.6185371841239</v>
       </c>
       <c r="N172" s="110">
         <f t="shared" ref="N172:Q172" si="98">N93</f>
-        <v>1506.8234188086776</v>
+        <v>1399.1816707803969</v>
       </c>
       <c r="O172" s="110">
         <f t="shared" si="98"/>
-        <v>1584.0964146450201</v>
+        <v>1412.8775671739427</v>
       </c>
       <c r="P172" s="110">
         <f t="shared" si="98"/>
-        <v>1657.5258838655441</v>
+        <v>1426.7075259140306</v>
       </c>
       <c r="Q172" s="110">
         <f t="shared" si="98"/>
-        <v>1802.982236939459</v>
+        <v>1440.6728592705722</v>
       </c>
     </row>
     <row r="173" spans="1:17" ht="16" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -20694,23 +20717,23 @@
       <c r="L174" s="111"/>
       <c r="M174" s="111">
         <f t="shared" ref="M174" si="102">SUM(M172)-SUM(M169:M171)</f>
-        <v>31.32129262134049</v>
+        <v>15.44662968413877</v>
       </c>
       <c r="N174" s="111">
         <f t="shared" ref="N174:Q174" si="103">SUM(N172)-SUM(N169:N171)</f>
-        <v>21.844108551721547</v>
+        <v>-19.077075649505332</v>
       </c>
       <c r="O174" s="111">
         <f t="shared" si="103"/>
-        <v>25.157357318817503</v>
+        <v>-56.62079332912981</v>
       </c>
       <c r="P174" s="111">
         <f t="shared" si="103"/>
-        <v>22.368696602727141</v>
+        <v>-97.404847478878537</v>
       </c>
       <c r="Q174" s="111">
         <f t="shared" si="103"/>
-        <v>64.713122544867019</v>
+        <v>-141.66528686502033</v>
       </c>
     </row>
     <row r="175" spans="1:17" ht="16" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -20742,23 +20765,23 @@
       <c r="L175" s="113"/>
       <c r="M175" s="110">
         <f>M174-H174</f>
-        <v>-45.67870737865951</v>
+        <v>-61.55337031586123</v>
       </c>
       <c r="N175" s="110">
         <f t="shared" ref="N175" si="105">N174-M174</f>
-        <v>-9.4771840696189429</v>
+        <v>-34.523705333644102</v>
       </c>
       <c r="O175" s="110">
         <f t="shared" ref="O175" si="106">O174-N174</f>
-        <v>3.3132487670959563</v>
+        <v>-37.543717679624478</v>
       </c>
       <c r="P175" s="110">
         <f t="shared" ref="P175" si="107">P174-O174</f>
-        <v>-2.7886607160903623</v>
+        <v>-40.784054149748727</v>
       </c>
       <c r="Q175" s="110">
         <f t="shared" ref="Q175" si="108">Q174-P174</f>
-        <v>42.344425942139878</v>
+        <v>-44.260439386141798</v>
       </c>
     </row>
     <row r="176" spans="1:17" ht="16" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -21664,10 +21687,22 @@
         <f>DATE(YEAR($C$205)+H206,MONTH($C$199),DAY($C$199))</f>
         <v>45291</v>
       </c>
-      <c r="I205" s="139"/>
-      <c r="J205" s="139"/>
-      <c r="K205" s="139"/>
-      <c r="L205" s="139"/>
+      <c r="I205" s="139">
+        <f t="shared" ref="I205:L205" si="119">DATE(YEAR($C$205)+I206,MONTH($C$199),DAY($C$199))</f>
+        <v>43830</v>
+      </c>
+      <c r="J205" s="139">
+        <f t="shared" si="119"/>
+        <v>43830</v>
+      </c>
+      <c r="K205" s="139">
+        <f t="shared" si="119"/>
+        <v>43830</v>
+      </c>
+      <c r="L205" s="139">
+        <f t="shared" si="119"/>
+        <v>43830</v>
+      </c>
       <c r="M205" s="139">
         <f>H205</f>
         <v>45291</v>
@@ -21679,7 +21714,7 @@
       <c r="P205" s="73"/>
       <c r="Q205" s="140">
         <f>H213*C197</f>
-        <v>57700.245575136243</v>
+        <v>79034.19825522165</v>
       </c>
       <c r="R205" s="76"/>
     </row>
@@ -21697,15 +21732,15 @@
         <v>1</v>
       </c>
       <c r="F206" s="132">
-        <f t="shared" ref="F206:H206" si="119">E206+1</f>
+        <f t="shared" ref="F206:H206" si="120">E206+1</f>
         <v>2</v>
       </c>
       <c r="G206" s="132">
-        <f t="shared" si="119"/>
+        <f t="shared" si="120"/>
         <v>3</v>
       </c>
       <c r="H206" s="132">
-        <f t="shared" si="119"/>
+        <f t="shared" si="120"/>
         <v>4</v>
       </c>
       <c r="I206" s="132"/>
@@ -21720,7 +21755,7 @@
       <c r="P206" s="76"/>
       <c r="Q206" s="130">
         <f>(H216*(1+$C$196))/(C195-C196)</f>
-        <v>34842.20779095577</v>
+        <v>51076.829392004052</v>
       </c>
       <c r="R206" s="76"/>
     </row>
@@ -21735,19 +21770,19 @@
         <v>1</v>
       </c>
       <c r="E207" s="133">
-        <f t="shared" ref="E207:H207" si="120">YEARFRAC(D205,E205)</f>
+        <f t="shared" ref="E207:H207" si="121">YEARFRAC(D205,E205)</f>
         <v>1</v>
       </c>
       <c r="F207" s="133">
-        <f t="shared" si="120"/>
+        <f t="shared" si="121"/>
         <v>1</v>
       </c>
       <c r="G207" s="133">
-        <f t="shared" si="120"/>
+        <f t="shared" si="121"/>
         <v>1</v>
       </c>
       <c r="H207" s="133">
-        <f t="shared" si="120"/>
+        <f t="shared" si="121"/>
         <v>1</v>
       </c>
       <c r="I207" s="133"/>
@@ -21764,7 +21799,7 @@
       <c r="P207" s="76"/>
       <c r="Q207" s="73">
         <f>AVERAGE(Q205:Q206)</f>
-        <v>46271.226683046007</v>
+        <v>65055.513823612855</v>
       </c>
       <c r="R207" s="76"/>
     </row>
@@ -21796,23 +21831,23 @@
       <c r="C209" s="76"/>
       <c r="D209" s="76">
         <f>M60+M54</f>
-        <v>4686.4973670475192</v>
+        <v>4472.9726402783817</v>
       </c>
       <c r="E209" s="76">
         <f>N60+N54</f>
-        <v>5615.6243144806394</v>
+        <v>5846.379172565059</v>
       </c>
       <c r="F209" s="76">
         <f>O60+O54</f>
-        <v>6424.1852272996839</v>
+        <v>7400.3237475837159</v>
       </c>
       <c r="G209" s="76">
         <f>P60+P54</f>
-        <v>7375.998032923002</v>
+        <v>9039.7384423633193</v>
       </c>
       <c r="H209" s="76">
         <f>Q60+Q54</f>
-        <v>7542.6703664437373</v>
+        <v>10824.816932610724</v>
       </c>
       <c r="I209" s="76"/>
       <c r="J209" s="76"/>
@@ -21833,23 +21868,23 @@
       <c r="C210" s="76"/>
       <c r="D210" s="130">
         <f>D209*$C$194</f>
-        <v>984.16444707997903</v>
+        <v>939.32425445846013</v>
       </c>
       <c r="E210" s="130">
         <f>E209*$C$194</f>
-        <v>1179.2811060409342</v>
+        <v>1227.7396262386624</v>
       </c>
       <c r="F210" s="130">
         <f>F209*$C$194</f>
-        <v>1349.0788977329337</v>
+        <v>1554.0679869925802</v>
       </c>
       <c r="G210" s="130">
         <f>G209*$C$194</f>
-        <v>1548.9595869138304</v>
+        <v>1898.3450728962971</v>
       </c>
       <c r="H210" s="130">
         <f>H209*$C$194</f>
-        <v>1583.9607769531847</v>
+        <v>2273.2115558482519</v>
       </c>
       <c r="I210" s="130"/>
       <c r="J210" s="130"/>
@@ -21873,23 +21908,23 @@
       <c r="C211" s="73"/>
       <c r="D211" s="140">
         <f>D209-D210</f>
-        <v>3702.33291996754</v>
+        <v>3533.6483858199217</v>
       </c>
       <c r="E211" s="140">
-        <f t="shared" ref="E211:H211" si="121">E209-E210</f>
-        <v>4436.3432084397054</v>
+        <f t="shared" ref="E211:H211" si="122">E209-E210</f>
+        <v>4618.6395463263962</v>
       </c>
       <c r="F211" s="140">
-        <f t="shared" si="121"/>
-        <v>5075.10632956675</v>
+        <f t="shared" si="122"/>
+        <v>5846.2557605911352</v>
       </c>
       <c r="G211" s="140">
-        <f t="shared" si="121"/>
-        <v>5827.0384460091718</v>
+        <f t="shared" si="122"/>
+        <v>7141.3933694670222</v>
       </c>
       <c r="H211" s="140">
-        <f t="shared" si="121"/>
-        <v>5958.7095894905524</v>
+        <f t="shared" si="122"/>
+        <v>8551.6053767624726</v>
       </c>
       <c r="I211" s="130"/>
       <c r="J211" s="130"/>
@@ -21953,23 +21988,23 @@
       <c r="C213" s="76"/>
       <c r="D213" s="130">
         <f>D209+D212</f>
-        <v>5960.1473670475189</v>
+        <v>5746.6226402783814</v>
       </c>
       <c r="E213" s="130">
-        <f t="shared" ref="E213:H213" si="122">E209+E212</f>
-        <v>6906.2505644806388</v>
+        <f t="shared" ref="E213:H213" si="123">E209+E212</f>
+        <v>7137.0054225650583</v>
       </c>
       <c r="F213" s="130">
-        <f t="shared" si="122"/>
-        <v>7730.5145085496833</v>
+        <f t="shared" si="123"/>
+        <v>8706.6530288337162</v>
       </c>
       <c r="G213" s="130">
-        <f t="shared" si="122"/>
-        <v>8696.8526180792524</v>
+        <f t="shared" si="123"/>
+        <v>10360.59302751957</v>
       </c>
       <c r="H213" s="130">
-        <f t="shared" si="122"/>
-        <v>8876.9608577132676</v>
+        <f t="shared" si="123"/>
+        <v>12159.107423880254</v>
       </c>
       <c r="I213" s="130"/>
       <c r="J213" s="130"/>
@@ -22037,23 +22072,23 @@
       <c r="C215" s="76"/>
       <c r="D215" s="76">
         <f>M175</f>
-        <v>-45.67870737865951</v>
+        <v>-61.55337031586123</v>
       </c>
       <c r="E215" s="76">
         <f>N175</f>
-        <v>-9.4771840696189429</v>
+        <v>-34.523705333644102</v>
       </c>
       <c r="F215" s="76">
         <f>O175</f>
-        <v>3.3132487670959563</v>
+        <v>-37.543717679624478</v>
       </c>
       <c r="G215" s="76">
         <f>P175</f>
-        <v>-2.7886607160903623</v>
+        <v>-40.784054149748727</v>
       </c>
       <c r="H215" s="76">
         <f>Q175</f>
-        <v>42.344425942139878</v>
+        <v>-44.260439386141798</v>
       </c>
       <c r="I215" s="76"/>
       <c r="J215" s="76"/>
@@ -22079,23 +22114,23 @@
       <c r="C216" s="74"/>
       <c r="D216" s="74">
         <f>D211+D212-D214-D215</f>
-        <v>3521.6616273461991</v>
+        <v>3368.8517561357826</v>
       </c>
       <c r="E216" s="74">
-        <f t="shared" ref="E216:H216" si="123">E211+E212-E214-E215</f>
-        <v>4236.4466425093251</v>
+        <f t="shared" ref="E216:L216" si="124">E211+E212-E214-E215</f>
+        <v>4443.7895016600396</v>
       </c>
       <c r="F216" s="74">
-        <f t="shared" si="123"/>
-        <v>4878.122362049653</v>
+        <f t="shared" si="124"/>
+        <v>5690.1287595207596</v>
       </c>
       <c r="G216" s="74">
-        <f t="shared" si="123"/>
-        <v>5650.6816918815111</v>
+        <f t="shared" si="124"/>
+        <v>7003.0320087730206</v>
       </c>
       <c r="H216" s="74">
-        <f t="shared" si="123"/>
-        <v>5750.6556548179433</v>
+        <f t="shared" si="124"/>
+        <v>8430.1563074181449</v>
       </c>
       <c r="I216" s="74"/>
       <c r="J216" s="74"/>
@@ -22103,7 +22138,7 @@
       <c r="L216" s="74"/>
       <c r="M216" s="141">
         <f>Q207</f>
-        <v>46271.226683046007</v>
+        <v>65055.513823612855</v>
       </c>
       <c r="N216" s="76"/>
       <c r="O216" s="76"/>
@@ -22151,31 +22186,43 @@
       </c>
       <c r="D218" s="144">
         <f>D216*D207</f>
-        <v>3521.6616273461991</v>
+        <v>3368.8517561357826</v>
       </c>
       <c r="E218" s="144">
-        <f t="shared" ref="E218:H218" si="124">E216*E207</f>
-        <v>4236.4466425093251</v>
+        <f t="shared" ref="E218:L218" si="125">E216*E207</f>
+        <v>4443.7895016600396</v>
       </c>
       <c r="F218" s="144">
-        <f t="shared" si="124"/>
-        <v>4878.122362049653</v>
+        <f t="shared" si="125"/>
+        <v>5690.1287595207596</v>
       </c>
       <c r="G218" s="144">
-        <f t="shared" si="124"/>
-        <v>5650.6816918815111</v>
+        <f t="shared" si="125"/>
+        <v>7003.0320087730206</v>
       </c>
       <c r="H218" s="144">
-        <f t="shared" si="124"/>
-        <v>5750.6556548179433</v>
-      </c>
-      <c r="I218" s="144"/>
-      <c r="J218" s="144"/>
-      <c r="K218" s="144"/>
-      <c r="L218" s="144"/>
+        <f t="shared" si="125"/>
+        <v>8430.1563074181449</v>
+      </c>
+      <c r="I218" s="144">
+        <f t="shared" si="125"/>
+        <v>0</v>
+      </c>
+      <c r="J218" s="144">
+        <f t="shared" si="125"/>
+        <v>0</v>
+      </c>
+      <c r="K218" s="144">
+        <f t="shared" si="125"/>
+        <v>0</v>
+      </c>
+      <c r="L218" s="144">
+        <f t="shared" si="125"/>
+        <v>0</v>
+      </c>
       <c r="M218" s="144">
         <f>M216*M207</f>
-        <v>46271.226683046007</v>
+        <v>65055.513823612855</v>
       </c>
       <c r="N218" s="79"/>
       <c r="O218" s="79"/>
@@ -22224,31 +22271,31 @@
       </c>
       <c r="D220" s="144">
         <f>D218</f>
-        <v>3521.6616273461991</v>
+        <v>3368.8517561357826</v>
       </c>
       <c r="E220" s="144">
-        <f t="shared" ref="E220:M220" si="125">E218</f>
-        <v>4236.4466425093251</v>
+        <f t="shared" ref="E220:M220" si="126">E218</f>
+        <v>4443.7895016600396</v>
       </c>
       <c r="F220" s="144">
-        <f t="shared" si="125"/>
-        <v>4878.122362049653</v>
+        <f t="shared" si="126"/>
+        <v>5690.1287595207596</v>
       </c>
       <c r="G220" s="144">
-        <f t="shared" si="125"/>
-        <v>5650.6816918815111</v>
+        <f t="shared" si="126"/>
+        <v>7003.0320087730206</v>
       </c>
       <c r="H220" s="144">
-        <f t="shared" si="125"/>
-        <v>5750.6556548179433</v>
+        <f t="shared" si="126"/>
+        <v>8430.1563074181449</v>
       </c>
       <c r="I220" s="144"/>
       <c r="J220" s="144"/>
       <c r="K220" s="144"/>
       <c r="L220" s="144"/>
       <c r="M220" s="144">
-        <f t="shared" si="125"/>
-        <v>46271.226683046007</v>
+        <f t="shared" si="126"/>
+        <v>65055.513823612855</v>
       </c>
       <c r="N220" s="79"/>
       <c r="O220" s="79"/>
@@ -22322,9 +22369,9 @@
         <v>170</v>
       </c>
       <c r="B223" s="148"/>
-      <c r="C223" s="482" t="e">
+      <c r="C223" s="482">
         <f>XNPV(C195,C218:M218,C205:M205)</f>
-        <v>#NUM!</v>
+        <v>42097.119139669448</v>
       </c>
       <c r="D223" s="79"/>
       <c r="E223" s="148" t="s">
@@ -22384,9 +22431,9 @@
         <v>173</v>
       </c>
       <c r="N224" s="79"/>
-      <c r="O224" s="150" t="e">
+      <c r="O224" s="150">
         <f>C228</f>
-        <v>#NUM!</v>
+        <v>80.579743757684696</v>
       </c>
       <c r="P224" s="79"/>
       <c r="Q224" s="79"/>
@@ -22424,9 +22471,9 @@
         <v>185</v>
       </c>
       <c r="N225" s="79"/>
-      <c r="O225" s="147" t="e">
+      <c r="O225" s="147">
         <f>O224/O223-1</f>
-        <v>#NUM!</v>
+        <v>0.46775489540409287</v>
       </c>
       <c r="P225" s="79"/>
       <c r="Q225" s="79"/>
@@ -22442,9 +22489,9 @@
         <v>47</v>
       </c>
       <c r="B226" s="79"/>
-      <c r="C226" s="148" t="e">
+      <c r="C226" s="148">
         <f>C223+C224-C225</f>
-        <v>#NUM!</v>
+        <v>42409.119139669448</v>
       </c>
       <c r="D226" s="79"/>
       <c r="E226" s="79" t="s">
@@ -22466,7 +22513,7 @@
       <c r="N226" s="79"/>
       <c r="O226" s="147">
         <f>XIRR(C220:M220,C205:M205)</f>
-        <v>0.23686266541481013</v>
+        <v>0.31594367623329156</v>
       </c>
       <c r="P226" s="79"/>
       <c r="Q226" s="79"/>
@@ -22507,9 +22554,9 @@
         <v>177</v>
       </c>
       <c r="B228" s="79"/>
-      <c r="C228" s="451" t="e">
+      <c r="C228" s="451">
         <f>C226/C201</f>
-        <v>#NUM!</v>
+        <v>80.579743757684696</v>
       </c>
       <c r="D228" s="79"/>
       <c r="E228" s="144" t="s">
@@ -22716,23 +22763,23 @@
       <c r="C235" s="108"/>
       <c r="D235" s="73">
         <f>D220</f>
-        <v>3521.6616273461991</v>
+        <v>3368.8517561357826</v>
       </c>
       <c r="E235" s="73">
         <f>E220</f>
-        <v>4236.4466425093251</v>
+        <v>4443.7895016600396</v>
       </c>
       <c r="F235" s="73">
         <f>F220</f>
-        <v>4878.122362049653</v>
+        <v>5690.1287595207596</v>
       </c>
       <c r="G235" s="73">
         <f>G220</f>
-        <v>5650.6816918815111</v>
+        <v>7003.0320087730206</v>
       </c>
       <c r="H235" s="73">
         <f>H220</f>
-        <v>5750.6556548179433</v>
+        <v>8430.1563074181449</v>
       </c>
       <c r="I235" s="76"/>
       <c r="J235" s="76"/>
@@ -22773,9 +22820,9 @@
         <v>180</v>
       </c>
       <c r="O236" s="64"/>
-      <c r="P236" s="135" t="e">
+      <c r="P236" s="135">
         <f>P237-P235</f>
-        <v>#NUM!</v>
+        <v>25.679743757684697</v>
       </c>
       <c r="Q236" s="64"/>
       <c r="R236" s="64"/>
@@ -22803,9 +22850,9 @@
         <v>167</v>
       </c>
       <c r="O237" s="64"/>
-      <c r="P237" s="135" t="e">
+      <c r="P237" s="135">
         <f>C228</f>
-        <v>#NUM!</v>
+        <v>80.579743757684696</v>
       </c>
       <c r="Q237" s="64"/>
       <c r="R237" s="64"/>
@@ -22996,8 +23043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V99"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="Q49" sqref="Q49"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -23111,7 +23158,7 @@
         <v>268</v>
       </c>
       <c r="L4" s="313">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M4" s="315"/>
     </row>
@@ -23180,7 +23227,7 @@
       <c r="H9" s="76"/>
       <c r="I9" s="391">
         <f>CHOOSE($L$4,I32,I55,I78)</f>
-        <v>2.5000000000000001E-2</v>
+        <v>-2.2672178274219957E-2</v>
       </c>
       <c r="J9" s="391">
         <f>CHOOSE($L$4,J32,J55,J78)</f>
@@ -23213,24 +23260,24 @@
       <c r="G10" s="76"/>
       <c r="H10" s="76"/>
       <c r="I10" s="76">
-        <f>CHOOSE($L$4,I33,I56,I79)</f>
-        <v>163790031.82499999</v>
+        <f t="shared" ref="I10:M10" si="1">CHOOSE($L$4,I33,I56,I79)</f>
+        <v>156172248.80382773</v>
       </c>
       <c r="J10" s="76">
-        <f>CHOOSE($L$4,J33,J56,J79)</f>
-        <v>167884782.62062496</v>
+        <f t="shared" si="1"/>
+        <v>160076555.02392343</v>
       </c>
       <c r="K10" s="76">
-        <f>CHOOSE($L$4,K33,K56,K79)</f>
-        <v>172081902.18614057</v>
+        <f t="shared" si="1"/>
+        <v>164078468.8995215</v>
       </c>
       <c r="L10" s="76">
-        <f>CHOOSE($L$4,L33,L56,L79)</f>
-        <v>176383949.74079406</v>
+        <f t="shared" si="1"/>
+        <v>168180430.62200952</v>
       </c>
       <c r="M10" s="76">
-        <f>CHOOSE($L$4,M33,M56,M79)</f>
-        <v>180793548.48431391</v>
+        <f t="shared" si="1"/>
+        <v>172384941.38755974</v>
       </c>
       <c r="N10" s="422"/>
       <c r="O10" s="76"/>
@@ -23247,23 +23294,23 @@
       <c r="G11" s="76"/>
       <c r="H11" s="76"/>
       <c r="I11" s="134">
-        <f>CHOOSE($L$4,I34,I57,I80)</f>
+        <f t="shared" ref="I11:M11" si="2">CHOOSE($L$4,I34,I57,I80)</f>
         <v>14.368749999999999</v>
       </c>
       <c r="J11" s="134">
-        <f>CHOOSE($L$4,J34,J57,J80)</f>
+        <f t="shared" si="2"/>
         <v>15.015343749999998</v>
       </c>
       <c r="K11" s="134">
-        <f>CHOOSE($L$4,K34,K57,K80)</f>
+        <f t="shared" si="2"/>
         <v>15.691034218749996</v>
       </c>
       <c r="L11" s="134">
-        <f>CHOOSE($L$4,L34,L57,L80)</f>
+        <f t="shared" si="2"/>
         <v>16.397130758593743</v>
       </c>
       <c r="M11" s="134">
-        <f>CHOOSE($L$4,M34,M57,M80)</f>
+        <f t="shared" si="2"/>
         <v>17.135001642730462</v>
       </c>
       <c r="N11" s="422"/>
@@ -23281,24 +23328,24 @@
       <c r="G12" s="76"/>
       <c r="H12" s="76"/>
       <c r="I12" s="134">
-        <f>CHOOSE($L$4,I35,I58,I81)</f>
-        <v>13.375999999999999</v>
+        <f t="shared" ref="I12:M12" si="3">CHOOSE($L$4,I35,I58,I81)</f>
+        <v>12.750194552529186</v>
       </c>
       <c r="J12" s="134">
-        <f>CHOOSE($L$4,J35,J58,J81)</f>
-        <v>13.977919999999999</v>
+        <f t="shared" si="3"/>
+        <v>12.700582900573821</v>
       </c>
       <c r="K12" s="134">
-        <f>CHOOSE($L$4,K35,K58,K81)</f>
-        <v>14.606926399999999</v>
+        <f t="shared" si="3"/>
+        <v>12.651164290065752</v>
       </c>
       <c r="L12" s="134">
-        <f>CHOOSE($L$4,L35,L58,L81)</f>
-        <v>15.264238087999997</v>
+        <f t="shared" si="3"/>
+        <v>12.601937969870946</v>
       </c>
       <c r="M12" s="134">
-        <f>CHOOSE($L$4,M35,M58,M81)</f>
-        <v>15.951128801959996</v>
+        <f t="shared" si="3"/>
+        <v>12.552903191778064</v>
       </c>
       <c r="N12" s="422"/>
       <c r="O12" s="76"/>
@@ -23315,24 +23362,24 @@
       <c r="G13" s="76"/>
       <c r="H13" s="76"/>
       <c r="I13" s="134">
-        <f>CHOOSE($L$4,I36,I59,I82)</f>
+        <f t="shared" ref="I13:M13" si="4">CHOOSE($L$4,I36,I59,I82)</f>
         <v>11.565772727272725</v>
       </c>
       <c r="J13" s="134">
-        <f>CHOOSE($L$4,J36,J59,J82)</f>
-        <v>11.7</v>
+        <f t="shared" si="4"/>
+        <v>11.394131071458736</v>
       </c>
       <c r="K13" s="134">
-        <f>CHOOSE($L$4,K36,K59,K82)</f>
-        <v>12</v>
+        <f t="shared" si="4"/>
+        <v>11.225036660753679</v>
       </c>
       <c r="L13" s="134">
-        <f>CHOOSE($L$4,L36,L59,L82)</f>
-        <v>12.25</v>
+        <f t="shared" si="4"/>
+        <v>11.058451692809319</v>
       </c>
       <c r="M13" s="134">
-        <f>CHOOSE($L$4,M36,M59,M82)</f>
-        <v>13</v>
+        <f t="shared" si="4"/>
+        <v>10.894338926282531</v>
       </c>
       <c r="N13" s="422"/>
       <c r="O13" s="83"/>
@@ -23350,23 +23397,23 @@
       <c r="G14" s="76"/>
       <c r="H14" s="76"/>
       <c r="I14" s="134">
-        <f>CHOOSE($L$4,I37,I60,I83)</f>
+        <f t="shared" ref="I14:M14" si="5">CHOOSE($L$4,I37,I60,I83)</f>
         <v>8.9384999999999994</v>
       </c>
       <c r="J14" s="134">
-        <f>CHOOSE($L$4,J37,J60,J83)</f>
+        <f t="shared" si="5"/>
         <v>9.0278849999999995</v>
       </c>
       <c r="K14" s="134">
-        <f>CHOOSE($L$4,K37,K60,K83)</f>
+        <f t="shared" si="5"/>
         <v>9.1181638500000002</v>
       </c>
       <c r="L14" s="134">
-        <f>CHOOSE($L$4,L37,L60,L83)</f>
+        <f t="shared" si="5"/>
         <v>9.2093454885000003</v>
       </c>
       <c r="M14" s="134">
-        <f>CHOOSE($L$4,M37,M60,M83)</f>
+        <f t="shared" si="5"/>
         <v>9.3014389433849995</v>
       </c>
       <c r="N14" s="424"/>
@@ -23385,24 +23432,24 @@
       <c r="G15" s="76"/>
       <c r="H15" s="76"/>
       <c r="I15" s="134">
-        <f>CHOOSE($L$4,I38,I61,I84)</f>
+        <f t="shared" ref="I15:M15" si="6">CHOOSE($L$4,I38,I61,I84)</f>
         <v>2.0499999999999998</v>
       </c>
       <c r="J15" s="134">
-        <f>CHOOSE($L$4,J38,J61,J84)</f>
-        <v>2.2000000000000002</v>
+        <f t="shared" si="6"/>
+        <v>2.0499999999999998</v>
       </c>
       <c r="K15" s="134">
-        <f>CHOOSE($L$4,K38,K61,K84)</f>
-        <v>2.2999999999999998</v>
+        <f t="shared" si="6"/>
+        <v>2.0499999999999998</v>
       </c>
       <c r="L15" s="134">
-        <f>CHOOSE($L$4,L38,L61,L84)</f>
-        <v>2.15</v>
+        <f t="shared" si="6"/>
+        <v>2.0499999999999998</v>
       </c>
       <c r="M15" s="134">
-        <f>CHOOSE($L$4,M38,M61,M84)</f>
-        <v>2.2999999999999998</v>
+        <f t="shared" si="6"/>
+        <v>2.0499999999999998</v>
       </c>
       <c r="N15" s="422"/>
       <c r="O15" s="76"/>
@@ -23420,23 +23467,23 @@
       <c r="G16" s="76"/>
       <c r="H16" s="76"/>
       <c r="I16" s="76">
-        <f>CHOOSE($L$4,I39,I62,I85)</f>
+        <f t="shared" ref="I16:M16" si="7">CHOOSE($L$4,I39,I62,I85)</f>
         <v>2099.1272371363634</v>
       </c>
       <c r="J16" s="76">
-        <f>CHOOSE($L$4,J39,J62,J85)</f>
+        <f t="shared" si="7"/>
         <v>2099.1272371363634</v>
       </c>
       <c r="K16" s="76">
-        <f>CHOOSE($L$4,K39,K62,K85)</f>
+        <f t="shared" si="7"/>
         <v>2099.1272371363634</v>
       </c>
       <c r="L16" s="76">
-        <f>CHOOSE($L$4,L39,L62,L85)</f>
+        <f t="shared" si="7"/>
         <v>2099.1272371363634</v>
       </c>
       <c r="M16" s="76">
-        <f>CHOOSE($L$4,M39,M62,M85)</f>
+        <f t="shared" si="7"/>
         <v>2099.1272371363634</v>
       </c>
       <c r="N16" s="422"/>
@@ -23455,23 +23502,23 @@
       <c r="G17" s="76"/>
       <c r="H17" s="76"/>
       <c r="I17" s="76">
-        <f>CHOOSE($L$4,I40,I63,I86)</f>
+        <f t="shared" ref="I17:M17" si="8">CHOOSE($L$4,I40,I63,I86)</f>
         <v>4303.210836129545</v>
       </c>
       <c r="J17" s="76">
-        <f>CHOOSE($L$4,J40,J63,J86)</f>
+        <f t="shared" si="8"/>
         <v>4303.210836129545</v>
       </c>
       <c r="K17" s="76">
-        <f>CHOOSE($L$4,K40,K63,K86)</f>
+        <f t="shared" si="8"/>
         <v>4303.210836129545</v>
       </c>
       <c r="L17" s="76">
-        <f>CHOOSE($L$4,L40,L63,L86)</f>
+        <f t="shared" si="8"/>
         <v>4303.210836129545</v>
       </c>
       <c r="M17" s="76">
-        <f>CHOOSE($L$4,M40,M63,M86)</f>
+        <f t="shared" si="8"/>
         <v>4303.210836129545</v>
       </c>
       <c r="N17" s="424"/>
@@ -23490,23 +23537,23 @@
       <c r="G18" s="316"/>
       <c r="H18" s="316"/>
       <c r="I18" s="304">
-        <f>CHOOSE($L$4,I41,I67,I90)</f>
+        <f t="shared" ref="I18:M18" si="9">CHOOSE($L$4,I41,I64,I87)</f>
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="J18" s="304">
-        <f>CHOOSE($L$4,J41,J67,J90)</f>
+        <f t="shared" si="9"/>
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="K18" s="304">
-        <f>CHOOSE($L$4,K41,K67,K90)</f>
+        <f t="shared" si="9"/>
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L18" s="304">
-        <f>CHOOSE($L$4,L41,L67,L90)</f>
+        <f t="shared" si="9"/>
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="M18" s="304">
-        <f>CHOOSE($L$4,M41,M67,M90)</f>
+        <f t="shared" si="9"/>
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="N18" s="422"/>
@@ -23525,23 +23572,23 @@
       <c r="G19" s="316"/>
       <c r="H19" s="316"/>
       <c r="I19" s="304">
-        <f>CHOOSE($L$4,I42,I68,I91)</f>
+        <f t="shared" ref="I19:M19" si="10">CHOOSE($L$4,I42,I65,I88)</f>
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="J19" s="304">
-        <f>CHOOSE($L$4,J42,J68,J91)</f>
+        <f t="shared" si="10"/>
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="K19" s="304">
-        <f>CHOOSE($L$4,K42,K68,K91)</f>
+        <f t="shared" si="10"/>
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="L19" s="304">
-        <f>CHOOSE($L$4,L42,L68,L91)</f>
+        <f t="shared" si="10"/>
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="M19" s="304">
-        <f>CHOOSE($L$4,M42,M68,M91)</f>
+        <f t="shared" si="10"/>
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="N19" s="422"/>
@@ -23560,23 +23607,23 @@
       <c r="G20" s="316"/>
       <c r="H20" s="316"/>
       <c r="I20" s="304">
-        <f>CHOOSE($L$4,I43,I69,I92)</f>
+        <f t="shared" ref="I20:M20" si="11">CHOOSE($L$4,I43,I66,I89)</f>
         <v>0.21</v>
       </c>
       <c r="J20" s="304">
-        <f>CHOOSE($L$4,J43,J69,J92)</f>
+        <f t="shared" si="11"/>
         <v>0.21</v>
       </c>
       <c r="K20" s="304">
-        <f>CHOOSE($L$4,K43,K69,K92)</f>
+        <f t="shared" si="11"/>
         <v>0.21</v>
       </c>
       <c r="L20" s="304">
-        <f>CHOOSE($L$4,L43,L69,L92)</f>
+        <f t="shared" si="11"/>
         <v>0.21</v>
       </c>
       <c r="M20" s="304">
-        <f>CHOOSE($L$4,M43,M69,M92)</f>
+        <f t="shared" si="11"/>
         <v>0.21</v>
       </c>
       <c r="N20" s="422"/>
@@ -23595,23 +23642,23 @@
       <c r="G21" s="316"/>
       <c r="H21" s="316"/>
       <c r="I21" s="307">
-        <f>CHOOSE($L$4,I44,I70,I93)</f>
+        <f t="shared" ref="I21:M21" si="12">CHOOSE($L$4,I44,I67,I90)</f>
         <v>10</v>
       </c>
       <c r="J21" s="307">
-        <f>CHOOSE($L$4,J44,J70,J93)</f>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
       <c r="K21" s="307">
-        <f>CHOOSE($L$4,K44,K70,K93)</f>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
       <c r="L21" s="307">
-        <f>CHOOSE($L$4,L44,L70,L93)</f>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
       <c r="M21" s="307">
-        <f>CHOOSE($L$4,M44,M70,M93)</f>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
       <c r="N21" s="422"/>
@@ -23630,23 +23677,23 @@
       <c r="G22" s="316"/>
       <c r="H22" s="316"/>
       <c r="I22" s="307">
-        <f>CHOOSE($L$4,I45,I71,I94)</f>
+        <f t="shared" ref="I22:M22" si="13">CHOOSE($L$4,I45,I68,I91)</f>
         <v>9</v>
       </c>
       <c r="J22" s="307">
-        <f>CHOOSE($L$4,J45,J71,J94)</f>
+        <f t="shared" si="13"/>
         <v>9</v>
       </c>
       <c r="K22" s="307">
-        <f>CHOOSE($L$4,K45,K71,K94)</f>
+        <f t="shared" si="13"/>
         <v>9</v>
       </c>
       <c r="L22" s="307">
-        <f>CHOOSE($L$4,L45,L71,L94)</f>
+        <f t="shared" si="13"/>
         <v>9</v>
       </c>
       <c r="M22" s="307">
-        <f>CHOOSE($L$4,M45,M71,M94)</f>
+        <f t="shared" si="13"/>
         <v>9</v>
       </c>
       <c r="N22" s="422"/>
@@ -23665,23 +23712,23 @@
       <c r="G23" s="316"/>
       <c r="H23" s="316"/>
       <c r="I23" s="307">
-        <f>CHOOSE($L$4,I46,I72,I95)</f>
+        <f t="shared" ref="I23:M23" si="14">CHOOSE($L$4,I46,I69,I92)</f>
         <v>108</v>
       </c>
       <c r="J23" s="307">
-        <f>CHOOSE($L$4,J46,J72,J95)</f>
+        <f t="shared" si="14"/>
         <v>108</v>
       </c>
       <c r="K23" s="307">
-        <f>CHOOSE($L$4,K46,K72,K95)</f>
+        <f t="shared" si="14"/>
         <v>108</v>
       </c>
       <c r="L23" s="307">
-        <f>CHOOSE($L$4,L46,L72,L95)</f>
+        <f t="shared" si="14"/>
         <v>108</v>
       </c>
       <c r="M23" s="307">
-        <f>CHOOSE($L$4,M46,M72,M95)</f>
+        <f t="shared" si="14"/>
         <v>108</v>
       </c>
       <c r="N23" s="422"/>
@@ -23700,23 +23747,23 @@
       <c r="G24" s="316"/>
       <c r="H24" s="316"/>
       <c r="I24" s="307">
-        <f>CHOOSE($L$4,I47,I73,I96)</f>
+        <f t="shared" ref="I24:M24" si="15">CHOOSE($L$4,I47,I70,I93)</f>
         <v>28</v>
       </c>
       <c r="J24" s="307">
-        <f>CHOOSE($L$4,J47,J73,J96)</f>
+        <f t="shared" si="15"/>
         <v>28</v>
       </c>
       <c r="K24" s="307">
-        <f>CHOOSE($L$4,K47,K73,K96)</f>
+        <f t="shared" si="15"/>
         <v>28</v>
       </c>
       <c r="L24" s="307">
-        <f>CHOOSE($L$4,L47,L73,L96)</f>
+        <f t="shared" si="15"/>
         <v>28</v>
       </c>
       <c r="M24" s="307">
-        <f>CHOOSE($L$4,M47,M73,M96)</f>
+        <f t="shared" si="15"/>
         <v>28</v>
       </c>
       <c r="N24" s="422"/>
@@ -23735,23 +23782,23 @@
       <c r="G25" s="316"/>
       <c r="H25" s="316"/>
       <c r="I25" s="307">
-        <f>CHOOSE($L$4,I48,I74,I97)</f>
+        <f t="shared" ref="I25:M25" si="16">CHOOSE($L$4,I48,I71,I94)</f>
         <v>1500</v>
       </c>
       <c r="J25" s="307">
-        <f>CHOOSE($L$4,J48,J74,J97)</f>
+        <f t="shared" si="16"/>
         <v>1500</v>
       </c>
       <c r="K25" s="307">
-        <f>CHOOSE($L$4,K48,K74,K97)</f>
+        <f t="shared" si="16"/>
         <v>1500</v>
       </c>
       <c r="L25" s="307">
-        <f>CHOOSE($L$4,L48,L74,L97)</f>
+        <f t="shared" si="16"/>
         <v>1500</v>
       </c>
       <c r="M25" s="307">
-        <f>CHOOSE($L$4,M48,M74,M97)</f>
+        <f t="shared" si="16"/>
         <v>1500</v>
       </c>
       <c r="N25" s="422"/>
@@ -23770,23 +23817,23 @@
       <c r="G26" s="316"/>
       <c r="H26" s="316"/>
       <c r="I26" s="307">
-        <f>CHOOSE($L$4,I49,I75,I98)</f>
+        <f t="shared" ref="I26:M26" si="17">CHOOSE($L$4,I49,I72,I95)</f>
         <v>-250</v>
       </c>
       <c r="J26" s="307">
-        <f>CHOOSE($L$4,J49,J75,J98)</f>
+        <f t="shared" si="17"/>
         <v>-250</v>
       </c>
       <c r="K26" s="307">
-        <f>CHOOSE($L$4,K49,K75,K98)</f>
+        <f t="shared" si="17"/>
         <v>-250</v>
       </c>
       <c r="L26" s="307">
-        <f>CHOOSE($L$4,L49,L75,L98)</f>
+        <f t="shared" si="17"/>
         <v>-250</v>
       </c>
       <c r="M26" s="307">
-        <f>CHOOSE($L$4,M49,M75,M98)</f>
+        <f t="shared" si="17"/>
         <v>-250</v>
       </c>
       <c r="N26" s="422"/>
@@ -23805,23 +23852,23 @@
       <c r="G27" s="316"/>
       <c r="H27" s="316"/>
       <c r="I27" s="307">
-        <f>CHOOSE($L$4,I50,I76,I99)</f>
+        <f t="shared" ref="I27:M27" si="18">CHOOSE($L$4,I50,I73,I96)</f>
         <v>-500</v>
       </c>
       <c r="J27" s="307">
-        <f>CHOOSE($L$4,J50,J76,J99)</f>
+        <f t="shared" si="18"/>
         <v>-500</v>
       </c>
       <c r="K27" s="307">
-        <f>CHOOSE($L$4,K50,K76,K99)</f>
+        <f t="shared" si="18"/>
         <v>-500</v>
       </c>
       <c r="L27" s="307">
-        <f>CHOOSE($L$4,L50,L76,L99)</f>
+        <f t="shared" si="18"/>
         <v>-500</v>
       </c>
       <c r="M27" s="307">
-        <f>CHOOSE($L$4,M50,M76,M99)</f>
+        <f t="shared" si="18"/>
         <v>-500</v>
       </c>
       <c r="N27" s="422"/>
@@ -23840,23 +23887,23 @@
       <c r="G28" s="316"/>
       <c r="H28" s="316"/>
       <c r="I28" s="307">
-        <f>CHOOSE($L$4,I51,#REF!,#REF!)</f>
+        <f t="shared" ref="I28:M28" si="19">CHOOSE($L$4,I51,I74,I97)</f>
         <v>-360</v>
       </c>
       <c r="J28" s="307">
-        <f>CHOOSE($L$4,J51,#REF!,#REF!)</f>
+        <f t="shared" si="19"/>
         <v>-360</v>
       </c>
       <c r="K28" s="307">
-        <f>CHOOSE($L$4,K51,#REF!,#REF!)</f>
+        <f t="shared" si="19"/>
         <v>-360</v>
       </c>
       <c r="L28" s="307">
-        <f>CHOOSE($L$4,L51,#REF!,#REF!)</f>
+        <f t="shared" si="19"/>
         <v>-360</v>
       </c>
       <c r="M28" s="307">
-        <f>CHOOSE($L$4,M51,#REF!,#REF!)</f>
+        <f t="shared" si="19"/>
         <v>-360</v>
       </c>
       <c r="N28" s="422"/>
@@ -23875,23 +23922,23 @@
       <c r="G29" s="316"/>
       <c r="H29" s="316"/>
       <c r="I29" s="306">
-        <f>CHOOSE($L$4,I52,#REF!,#REF!)</f>
+        <f t="shared" ref="I29:M29" si="20">CHOOSE($L$4,I52,I75,I98)</f>
         <v>0.2</v>
       </c>
       <c r="J29" s="306">
-        <f>CHOOSE($L$4,J52,#REF!,#REF!)</f>
+        <f t="shared" si="20"/>
         <v>0.2</v>
       </c>
       <c r="K29" s="306">
-        <f>CHOOSE($L$4,K52,#REF!,#REF!)</f>
+        <f t="shared" si="20"/>
         <v>0.2</v>
       </c>
       <c r="L29" s="306">
-        <f>CHOOSE($L$4,L52,#REF!,#REF!)</f>
+        <f t="shared" si="20"/>
         <v>0.2</v>
       </c>
       <c r="M29" s="306">
-        <f>CHOOSE($L$4,M52,#REF!,#REF!)</f>
+        <f t="shared" si="20"/>
         <v>0.2</v>
       </c>
       <c r="N29" s="76"/>
@@ -23903,23 +23950,23 @@
         <v>461</v>
       </c>
       <c r="I30" s="306">
-        <f>CHOOSE($L$4,I53,#REF!,#REF!)</f>
+        <f t="shared" ref="I30:M30" si="21">CHOOSE($L$4,I53,I76,I99)</f>
         <v>0.8</v>
       </c>
       <c r="J30" s="306">
-        <f>CHOOSE($L$4,J53,#REF!,#REF!)</f>
+        <f t="shared" si="21"/>
         <v>0.8</v>
       </c>
       <c r="K30" s="306">
-        <f>CHOOSE($L$4,K53,#REF!,#REF!)</f>
+        <f t="shared" si="21"/>
         <v>0.8</v>
       </c>
       <c r="L30" s="306">
-        <f>CHOOSE($L$4,L53,#REF!,#REF!)</f>
+        <f t="shared" si="21"/>
         <v>0.8</v>
       </c>
       <c r="M30" s="306">
-        <f>CHOOSE($L$4,M53,#REF!,#REF!)</f>
+        <f t="shared" si="21"/>
         <v>0.8</v>
       </c>
       <c r="N30" s="76"/>
@@ -23996,18 +24043,23 @@
         <v>159795153</v>
       </c>
       <c r="I33" s="76">
+        <f>H33*(1+I32)</f>
         <v>163790031.82499999</v>
       </c>
       <c r="J33" s="76">
+        <f t="shared" ref="J33" si="22">I33*(1+J32)</f>
         <v>167884782.62062496</v>
       </c>
       <c r="K33" s="76">
+        <f t="shared" ref="K33" si="23">J33*(1+K32)</f>
         <v>172081902.18614057</v>
       </c>
       <c r="L33" s="76">
+        <f t="shared" ref="L33" si="24">K33*(1+L32)</f>
         <v>176383949.74079406</v>
       </c>
       <c r="M33" s="76">
+        <f t="shared" ref="M33" si="25">L33*(1+M32)</f>
         <v>180793548.48431391</v>
       </c>
       <c r="N33" s="422"/>
@@ -24068,19 +24120,19 @@
         <v>13.375999999999999</v>
       </c>
       <c r="J35" s="134">
-        <f t="shared" ref="J35:M35" si="1">I35*(J34/I34)</f>
+        <f t="shared" ref="J35:M35" si="26">I35*(J34/I34)</f>
         <v>13.977919999999999</v>
       </c>
       <c r="K35" s="134">
-        <f t="shared" si="1"/>
+        <f t="shared" si="26"/>
         <v>14.606926399999999</v>
       </c>
       <c r="L35" s="134">
-        <f t="shared" si="1"/>
+        <f t="shared" si="26"/>
         <v>15.264238087999997</v>
       </c>
       <c r="M35" s="134">
-        <f t="shared" si="1"/>
+        <f t="shared" si="26"/>
         <v>15.951128801959996</v>
       </c>
       <c r="N35" s="422"/>
@@ -24629,19 +24681,19 @@
         <v>0.8</v>
       </c>
       <c r="J53" s="306">
-        <f t="shared" ref="J53" si="2">1-J52</f>
+        <f t="shared" ref="J53" si="27">1-J52</f>
         <v>0.8</v>
       </c>
       <c r="K53" s="306">
-        <f t="shared" ref="K53" si="3">1-K52</f>
+        <f t="shared" ref="K53" si="28">1-K52</f>
         <v>0.8</v>
       </c>
       <c r="L53" s="306">
-        <f t="shared" ref="L53" si="4">1-L52</f>
+        <f t="shared" ref="L53" si="29">1-L52</f>
         <v>0.8</v>
       </c>
       <c r="M53" s="306">
-        <f t="shared" ref="M53" si="5">1-M52</f>
+        <f t="shared" ref="M53" si="30">1-M52</f>
         <v>0.8</v>
       </c>
       <c r="N53" s="76"/>
@@ -24701,8 +24753,7 @@
         <v>3.8905398175756778E-2</v>
       </c>
       <c r="I55" s="391">
-        <f>Analysis!J2</f>
-        <v>2.5000000000000001E-2</v>
+        <v>-2.2672178274219957E-2</v>
       </c>
       <c r="J55" s="391">
         <f>Analysis!K2</f>
@@ -24763,24 +24814,24 @@
         <v>159795153</v>
       </c>
       <c r="I56" s="76">
-        <f>Analysis!J13</f>
-        <v>163790031.82499999</v>
+        <f>H56*(1+I55)</f>
+        <v>156172248.80382773</v>
       </c>
       <c r="J56" s="76">
-        <f>Analysis!K13</f>
-        <v>167884782.62062496</v>
+        <f t="shared" ref="J56:M56" si="31">I56*(1+J55)</f>
+        <v>160076555.02392343</v>
       </c>
       <c r="K56" s="76">
-        <f>Analysis!L13</f>
-        <v>172081902.18614057</v>
+        <f t="shared" si="31"/>
+        <v>164078468.8995215</v>
       </c>
       <c r="L56" s="76">
-        <f>Analysis!M13</f>
-        <v>176383949.74079406</v>
+        <f t="shared" si="31"/>
+        <v>168180430.62200952</v>
       </c>
       <c r="M56" s="76">
-        <f>Analysis!N13</f>
-        <v>180793548.48431391</v>
+        <f t="shared" si="31"/>
+        <v>172384941.38755974</v>
       </c>
       <c r="N56" s="422" t="s">
         <v>497</v>
@@ -25130,25 +25181,20 @@
       <c r="A64" s="422" t="s">
         <v>449</v>
       </c>
-      <c r="I64" s="421">
-        <f>I$56*I60/100000</f>
-        <v>14640.371994677622</v>
-      </c>
-      <c r="J64" s="421">
-        <f>J$56*J60/100000</f>
-        <v>15156.445107490008</v>
-      </c>
-      <c r="K64" s="421">
-        <f>K$56*K60/100000</f>
-        <v>15690.709797529029</v>
-      </c>
-      <c r="L64" s="421">
-        <f>L$56*L60/100000</f>
-        <v>16243.807317891928</v>
-      </c>
-      <c r="M64" s="421">
-        <f>M$56*M60/100000</f>
-        <v>16816.401525847614</v>
+      <c r="I64" s="304">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="J64" s="304">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="K64" s="304">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="L64" s="304">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="M64" s="304">
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="N64" s="422"/>
     </row>
@@ -25163,20 +25209,20 @@
       <c r="F65" s="472"/>
       <c r="G65" s="472"/>
       <c r="H65" s="472"/>
-      <c r="I65" s="305" t="s">
-        <v>265</v>
-      </c>
-      <c r="J65" s="305" t="s">
-        <v>265</v>
-      </c>
-      <c r="K65" s="305" t="s">
-        <v>265</v>
-      </c>
-      <c r="L65" s="305" t="s">
-        <v>265</v>
-      </c>
-      <c r="M65" s="305" t="s">
-        <v>265</v>
+      <c r="I65" s="304">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="J65" s="304">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="K65" s="304">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="L65" s="304">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="M65" s="304">
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="N65" s="422"/>
     </row>
@@ -25191,25 +25237,20 @@
       <c r="F66" s="472"/>
       <c r="G66" s="472"/>
       <c r="H66" s="472"/>
-      <c r="I66" s="304" t="e">
-        <f>#REF!*0.95</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J66" s="304" t="e">
-        <f>#REF!*0.95</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K66" s="304" t="e">
-        <f>#REF!*0.95</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L66" s="304" t="e">
-        <f>#REF!*0.95</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M66" s="304" t="e">
-        <f>#REF!*0.95</f>
-        <v>#REF!</v>
+      <c r="I66" s="304">
+        <v>0.21</v>
+      </c>
+      <c r="J66" s="304">
+        <v>0.21</v>
+      </c>
+      <c r="K66" s="304">
+        <v>0.21</v>
+      </c>
+      <c r="L66" s="304">
+        <v>0.21</v>
+      </c>
+      <c r="M66" s="304">
+        <v>0.21</v>
       </c>
       <c r="N66" s="422"/>
     </row>
@@ -25217,25 +25258,20 @@
       <c r="A67" s="422" t="s">
         <v>452</v>
       </c>
-      <c r="I67" s="304">
-        <f>I41*2</f>
-        <v>0.15</v>
-      </c>
-      <c r="J67" s="304">
-        <f>J41*2</f>
-        <v>0.15</v>
-      </c>
-      <c r="K67" s="304">
-        <f>K41*2</f>
-        <v>0.15</v>
-      </c>
-      <c r="L67" s="304">
-        <f>L41*2</f>
-        <v>0.15</v>
-      </c>
-      <c r="M67" s="304">
-        <f>M41*2</f>
-        <v>0.15</v>
+      <c r="I67" s="307">
+        <v>10</v>
+      </c>
+      <c r="J67" s="307">
+        <v>10</v>
+      </c>
+      <c r="K67" s="307">
+        <v>10</v>
+      </c>
+      <c r="L67" s="307">
+        <v>10</v>
+      </c>
+      <c r="M67" s="307">
+        <v>10</v>
       </c>
       <c r="N67" s="422"/>
     </row>
@@ -25243,20 +25279,20 @@
       <c r="A68" s="422" t="s">
         <v>453</v>
       </c>
-      <c r="I68" s="304">
-        <v>0.01</v>
-      </c>
-      <c r="J68" s="304">
-        <v>0.01</v>
-      </c>
-      <c r="K68" s="304">
-        <v>0.01</v>
-      </c>
-      <c r="L68" s="304">
-        <v>0.01</v>
-      </c>
-      <c r="M68" s="304">
-        <v>0.01</v>
+      <c r="I68" s="307">
+        <v>9</v>
+      </c>
+      <c r="J68" s="307">
+        <v>9</v>
+      </c>
+      <c r="K68" s="307">
+        <v>9</v>
+      </c>
+      <c r="L68" s="307">
+        <v>9</v>
+      </c>
+      <c r="M68" s="307">
+        <v>9</v>
       </c>
       <c r="N68" s="422"/>
     </row>
@@ -25264,25 +25300,20 @@
       <c r="A69" s="422" t="s">
         <v>454</v>
       </c>
-      <c r="I69" s="304">
-        <f>I43*2</f>
-        <v>0.42</v>
-      </c>
-      <c r="J69" s="304">
-        <f>J43*2</f>
-        <v>0.42</v>
-      </c>
-      <c r="K69" s="304">
-        <f>K43*2</f>
-        <v>0.42</v>
-      </c>
-      <c r="L69" s="304">
-        <f>L43*2</f>
-        <v>0.42</v>
-      </c>
-      <c r="M69" s="304">
-        <f>M43*2</f>
-        <v>0.42</v>
+      <c r="I69" s="307">
+        <v>108</v>
+      </c>
+      <c r="J69" s="307">
+        <v>108</v>
+      </c>
+      <c r="K69" s="307">
+        <v>108</v>
+      </c>
+      <c r="L69" s="307">
+        <v>108</v>
+      </c>
+      <c r="M69" s="307">
+        <v>108</v>
       </c>
       <c r="N69" s="422"/>
     </row>
@@ -25291,19 +25322,19 @@
         <v>455</v>
       </c>
       <c r="I70" s="307">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J70" s="307">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="K70" s="307">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="L70" s="307">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="M70" s="307">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="N70" s="422"/>
     </row>
@@ -25312,19 +25343,19 @@
         <v>456</v>
       </c>
       <c r="I71" s="307">
-        <v>120</v>
+        <v>1500</v>
       </c>
       <c r="J71" s="307">
-        <v>120</v>
+        <v>1500</v>
       </c>
       <c r="K71" s="307">
-        <v>120</v>
+        <v>1500</v>
       </c>
       <c r="L71" s="307">
-        <v>120</v>
+        <v>1500</v>
       </c>
       <c r="M71" s="307">
-        <v>120</v>
+        <v>1500</v>
       </c>
       <c r="N71" s="422"/>
     </row>
@@ -25333,19 +25364,19 @@
         <v>457</v>
       </c>
       <c r="I72" s="307">
-        <v>22</v>
+        <v>-250</v>
       </c>
       <c r="J72" s="307">
-        <v>22</v>
+        <v>-250</v>
       </c>
       <c r="K72" s="307">
-        <v>22</v>
+        <v>-250</v>
       </c>
       <c r="L72" s="307">
-        <v>22</v>
+        <v>-250</v>
       </c>
       <c r="M72" s="307">
-        <v>22</v>
+        <v>-250</v>
       </c>
       <c r="N72" s="422"/>
     </row>
@@ -25354,19 +25385,19 @@
         <v>458</v>
       </c>
       <c r="I73" s="307">
-        <v>32</v>
+        <v>-500</v>
       </c>
       <c r="J73" s="307">
-        <v>32</v>
+        <v>-500</v>
       </c>
       <c r="K73" s="307">
-        <v>32</v>
+        <v>-500</v>
       </c>
       <c r="L73" s="307">
-        <v>32</v>
+        <v>-500</v>
       </c>
       <c r="M73" s="307">
-        <v>32</v>
+        <v>-500</v>
       </c>
       <c r="N73" s="422"/>
     </row>
@@ -25375,19 +25406,19 @@
         <v>459</v>
       </c>
       <c r="I74" s="307">
-        <v>1500</v>
+        <v>-360</v>
       </c>
       <c r="J74" s="307">
-        <v>1500</v>
+        <v>-360</v>
       </c>
       <c r="K74" s="307">
-        <v>1500</v>
+        <v>-360</v>
       </c>
       <c r="L74" s="307">
-        <v>1500</v>
+        <v>-360</v>
       </c>
       <c r="M74" s="307">
-        <v>1500</v>
+        <v>-360</v>
       </c>
       <c r="N74" s="422"/>
     </row>
@@ -25421,19 +25452,19 @@
         <v>0.8</v>
       </c>
       <c r="J76" s="306">
-        <f t="shared" ref="J76:M76" si="6">1-J75</f>
+        <f t="shared" ref="J76" si="32">1-J75</f>
         <v>0.8</v>
       </c>
       <c r="K76" s="306">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="K76" si="33">1-K75</f>
         <v>0.8</v>
       </c>
       <c r="L76" s="306">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="L76" si="34">1-L75</f>
         <v>0.8</v>
       </c>
       <c r="M76" s="306">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="M76" si="35">1-M75</f>
         <v>0.8</v>
       </c>
       <c r="N76" s="76"/>
@@ -25503,18 +25534,23 @@
         <v>159795153</v>
       </c>
       <c r="I79" s="76">
+        <f>H79*(1+I78)</f>
         <v>163790031.82499999</v>
       </c>
       <c r="J79" s="76">
+        <f t="shared" ref="J79" si="36">I79*(1+J78)</f>
         <v>167884782.62062496</v>
       </c>
       <c r="K79" s="76">
+        <f t="shared" ref="K79" si="37">J79*(1+K78)</f>
         <v>172081902.18614057</v>
       </c>
       <c r="L79" s="76">
+        <f t="shared" ref="L79" si="38">K79*(1+L78)</f>
         <v>176383949.74079406</v>
       </c>
       <c r="M79" s="76">
+        <f t="shared" ref="M79" si="39">L79*(1+M78)</f>
         <v>180793548.48431391</v>
       </c>
       <c r="N79" s="424"/>

</xml_diff>